<commit_message>
test(aperturas_masivas.xlsx): testing endpoint to process xlsx file and retrive data
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Desktop/personal-projects/APA-BACKEND/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A91C7919-2F3A-AE42-A1B3-EEA7E4F66DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B071F65C-A41E-3249-8F58-9F05E999F199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{9017CD1B-9B7B-4744-9A02-2681E840ED07}"/>
   </bookViews>
@@ -36,33 +36,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>COL1</t>
-  </si>
-  <si>
-    <t>COL2</t>
-  </si>
-  <si>
-    <t>COL3</t>
-  </si>
-  <si>
-    <t>data1</t>
-  </si>
-  <si>
-    <t>data2</t>
-  </si>
-  <si>
-    <t>data3</t>
-  </si>
-  <si>
-    <t>data4</t>
-  </si>
-  <si>
-    <t>data5</t>
-  </si>
-  <si>
-    <t>data6</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+  <si>
+    <t>Recaudadora</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Cuenta</t>
+  </si>
+  <si>
+    <t>Fecha de otorgamiento</t>
+  </si>
+  <si>
+    <t>Recamaras</t>
+  </si>
+  <si>
+    <t>Banios</t>
+  </si>
+  <si>
+    <t>Localidad</t>
+  </si>
+  <si>
+    <t>Colonia</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>San Agustin</t>
+  </si>
+  <si>
+    <t>El Palomar</t>
+  </si>
+  <si>
+    <t>Tlajo</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>12/04/2023</t>
   </si>
 </sst>
 </file>
@@ -105,9 +120,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,15 +462,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0249D18-3148-3041-AACF-08B1B08C8CC5}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="18.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23" style="2" customWidth="1"/>
+    <col min="5" max="7" width="18.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -460,27 +487,98 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>93</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2">
+        <v>123456</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>77</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>8877</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>132</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4455</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
+      <c r="F4" s="2">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>